<commit_message>
feat: expand arcane depths ui integration
</commit_message>
<xml_diff>
--- a/example/game_04_arcane_depths/rooms.xlsx
+++ b/example/game_04_arcane_depths/rooms.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -659,40 +659,40 @@
         <v>50</v>
       </c>
       <c r="B7" t="str">
+        <v>04</v>
+      </c>
+      <c r="C7" t="str">
         <v>01</v>
       </c>
-      <c r="C7" t="str">
-        <v>02</v>
-      </c>
       <c r="D7" t="str">
         <v>00</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="str">
-        <v>Combat</v>
+        <v>Elite</v>
       </c>
       <c r="G7" t="str">
-        <v>蔓生之巢</v>
+        <v>熔核军械库</v>
       </c>
       <c r="H7">
-        <v>10020100</v>
+        <v>10010100</v>
       </c>
       <c r="I7" t="str">
-        <v>藤蔓潮汐的核心据点。</v>
+        <v>对抗熔核巨灵与其护卫。</v>
       </c>
       <c r="J7">
-        <v>40020300</v>
+        <v>40010200</v>
       </c>
       <c r="L7" t="str">
-        <v>Resource</v>
+        <v>Relic</v>
       </c>
       <c r="M7" t="str">
-        <v>Provision:18</v>
+        <v>60010000</v>
       </c>
       <c r="N7" t="str">
-        <v>初始时所有敌人持有藤蔓护盾</v>
+        <v>精英常驻熔火护盾，每回合爆发灼烧波</v>
       </c>
     </row>
     <row r="8">
@@ -700,37 +700,40 @@
         <v>50</v>
       </c>
       <c r="B8" t="str">
-        <v>05</v>
+        <v>06</v>
       </c>
       <c r="C8" t="str">
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="D8" t="str">
         <v>00</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" t="str">
-        <v>Rest</v>
+        <v>Boss</v>
       </c>
       <c r="G8" t="str">
-        <v>翠息静室</v>
+        <v>灰烬之主燃殿</v>
       </c>
       <c r="H8">
-        <v>10020100</v>
+        <v>10010100</v>
       </c>
       <c r="I8" t="str">
-        <v>通过深绿脉络恢复与净化。</v>
+        <v>灰烬之主统御火种，终焉决战即将开启。</v>
+      </c>
+      <c r="J8">
+        <v>40010300</v>
       </c>
       <c r="L8" t="str">
-        <v>Trait</v>
+        <v>Relic</v>
       </c>
       <c r="M8" t="str">
-        <v>Synergy</v>
+        <v>60010000</v>
       </c>
       <c r="N8" t="str">
-        <v>移除任意一个减益</v>
+        <v>Boss首次登场时施加全场灼烧</v>
       </c>
     </row>
     <row r="9">
@@ -738,45 +741,288 @@
         <v>50</v>
       </c>
       <c r="B9" t="str">
+        <v>01</v>
+      </c>
+      <c r="C9" t="str">
+        <v>02</v>
+      </c>
+      <c r="D9" t="str">
+        <v>00</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Combat</v>
+      </c>
+      <c r="G9" t="str">
+        <v>蔓生之巢</v>
+      </c>
+      <c r="H9">
+        <v>10020100</v>
+      </c>
+      <c r="I9" t="str">
+        <v>藤蔓潮汐的核心据点。</v>
+      </c>
+      <c r="J9">
+        <v>40020300</v>
+      </c>
+      <c r="L9" t="str">
+        <v>Resource</v>
+      </c>
+      <c r="M9" t="str">
+        <v>Provision:18</v>
+      </c>
+      <c r="N9" t="str">
+        <v>初始时所有敌人持有藤蔓护盾</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>50</v>
+      </c>
+      <c r="B10" t="str">
+        <v>02</v>
+      </c>
+      <c r="C10" t="str">
+        <v>02</v>
+      </c>
+      <c r="D10" t="str">
+        <v>00</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Event</v>
+      </c>
+      <c r="G10" t="str">
+        <v>深根共鸣</v>
+      </c>
+      <c r="H10">
+        <v>10020100</v>
+      </c>
+      <c r="I10" t="str">
+        <v>旅者请求帮助，分享绿色共鸣。</v>
+      </c>
+      <c r="K10">
+        <v>51020000</v>
+      </c>
+      <c r="L10" t="str">
+        <v>Resource</v>
+      </c>
+      <c r="M10" t="str">
+        <v>Provision:15</v>
+      </c>
+      <c r="N10" t="str">
+        <v>成功则提升当前层的治愈效率</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>50</v>
+      </c>
+      <c r="B11" t="str">
+        <v>05</v>
+      </c>
+      <c r="C11" t="str">
+        <v>01</v>
+      </c>
+      <c r="D11" t="str">
+        <v>00</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Rest</v>
+      </c>
+      <c r="G11" t="str">
+        <v>翠息静室</v>
+      </c>
+      <c r="H11">
+        <v>10020100</v>
+      </c>
+      <c r="I11" t="str">
+        <v>通过深绿脉络恢复与净化。</v>
+      </c>
+      <c r="L11" t="str">
+        <v>Trait</v>
+      </c>
+      <c r="M11" t="str">
+        <v>Synergy</v>
+      </c>
+      <c r="N11" t="str">
+        <v>移除任意一个减益</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>50</v>
+      </c>
+      <c r="B12" t="str">
         <v>06</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C12" t="str">
+        <v>03</v>
+      </c>
+      <c r="D12" t="str">
+        <v>00</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Boss</v>
+      </c>
+      <c r="G12" t="str">
+        <v>藤界之心</v>
+      </c>
+      <c r="H12">
+        <v>10020100</v>
+      </c>
+      <c r="I12" t="str">
+        <v>削弱深根巨树的束缚并阻止其觉醒。</v>
+      </c>
+      <c r="J12">
+        <v>40020300</v>
+      </c>
+      <c r="L12" t="str">
+        <v>Relic</v>
+      </c>
+      <c r="M12" t="str">
+        <v>60020000</v>
+      </c>
+      <c r="N12" t="str">
+        <v>Boss召唤孢子爪牙并周期性缠绕全队</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>50</v>
+      </c>
+      <c r="B13" t="str">
         <v>01</v>
       </c>
-      <c r="D9" t="str">
-        <v>00</v>
-      </c>
-      <c r="E9">
+      <c r="C13" t="str">
+        <v>03</v>
+      </c>
+      <c r="D13" t="str">
+        <v>00</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Combat</v>
+      </c>
+      <c r="G13" t="str">
+        <v>星火熔层</v>
+      </c>
+      <c r="H13">
+        <v>10030100</v>
+      </c>
+      <c r="I13" t="str">
+        <v>熔炉中游走的星火构装体。</v>
+      </c>
+      <c r="J13">
+        <v>40030100</v>
+      </c>
+      <c r="L13" t="str">
+        <v>Resource</v>
+      </c>
+      <c r="M13" t="str">
+        <v>Arcane:16</v>
+      </c>
+      <c r="N13" t="str">
+        <v>地图施加减速并周期性落下星火</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>50</v>
+      </c>
+      <c r="B14" t="str">
+        <v>04</v>
+      </c>
+      <c r="C14" t="str">
+        <v>02</v>
+      </c>
+      <c r="D14" t="str">
+        <v>00</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Elite</v>
+      </c>
+      <c r="G14" t="str">
+        <v>星界锻卫</v>
+      </c>
+      <c r="H14">
+        <v>10030100</v>
+      </c>
+      <c r="I14" t="str">
+        <v>星界傀儡组成的防线。</v>
+      </c>
+      <c r="J14">
+        <v>40030100</v>
+      </c>
+      <c r="L14" t="str">
+        <v>Relic</v>
+      </c>
+      <c r="M14" t="str">
+        <v>60030000</v>
+      </c>
+      <c r="N14" t="str">
+        <v>精英拥有反射护盾与星能回复</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>50</v>
+      </c>
+      <c r="B15" t="str">
+        <v>06</v>
+      </c>
+      <c r="C15" t="str">
+        <v>01</v>
+      </c>
+      <c r="D15" t="str">
+        <v>00</v>
+      </c>
+      <c r="E15">
         <v>1</v>
       </c>
-      <c r="F9" t="str">
+      <c r="F15" t="str">
         <v>Boss</v>
       </c>
-      <c r="G9" t="str">
+      <c r="G15" t="str">
         <v>熔炉主宰之厅</v>
       </c>
-      <c r="H9">
+      <c r="H15">
         <v>10030100</v>
       </c>
-      <c r="I9" t="str">
+      <c r="I15" t="str">
         <v>对决星界熔炉的主宰。</v>
       </c>
-      <c r="J9">
+      <c r="J15">
         <v>40030300</v>
       </c>
-      <c r="L9" t="str">
+      <c r="L15" t="str">
         <v>Relic</v>
       </c>
-      <c r="M9" t="str">
+      <c r="M15" t="str">
         <v>60030000</v>
       </c>
-      <c r="N9" t="str">
+      <c r="N15" t="str">
         <v>Boss阶段转换召唤星火残迹</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>